<commit_message>
Hypothesis testing symbols. Article plan updated
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33FDC39-456C-4380-86A5-BDB65A2BDEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85783BB0-5ED3-4746-A0E7-8A76705BC772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Others/contingency</t>
   </si>
   <si>
-    <t>End</t>
-  </si>
-  <si>
     <t>Updated with 7-Jul results</t>
   </si>
   <si>
@@ -150,17 +147,26 @@
     <t>Super models: Results</t>
   </si>
   <si>
-    <t>TO DO</t>
-  </si>
-  <si>
     <t>Table to be updated for Fbeta</t>
+  </si>
+  <si>
+    <t>Statistical tests</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Planned end</t>
+  </si>
+  <si>
+    <t>Shifted End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +192,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -322,39 +334,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,16 +380,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>546652</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>236800</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>584669</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>161525</xdr:rowOff>
+      <xdr:rowOff>37286</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -414,8 +412,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6877050" y="847725"/>
-          <a:ext cx="10600000" cy="3200000"/>
+          <a:off x="9831456" y="728870"/>
+          <a:ext cx="10656322" cy="3168112"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -690,35 +688,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="8" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="23">
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="28">
+        <v>45110</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="28">
+        <f>F1+31</f>
         <v>45141</v>
       </c>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -738,217 +746,212 @@
       <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="25">
+        <f ca="1">TODAY()+D36</f>
+        <v>45147.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
       <c r="E3" s="14">
         <v>45110</v>
       </c>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="14">
         <v>45110</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="23">
         <v>45115</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="23">
+        <v>45115</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="14">
+        <v>45110</v>
+      </c>
+      <c r="F6" s="23">
+        <v>45115</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="25">
+      <c r="E7" s="14"/>
+      <c r="F7" s="23">
         <v>45115</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29">
-        <v>45110</v>
-      </c>
-      <c r="F6" s="31">
+    </row>
+    <row r="8" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="23">
         <v>45115</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="30" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="31">
+      <c r="D9" s="19"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22">
         <v>45115</v>
       </c>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="G9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
+    </row>
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="D10" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>2.1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="20">
+      <c r="D11" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+    <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
         <v>3.1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="D14" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
         <v>3.2</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="D15" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
         <v>3.3</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="20">
+      <c r="D16" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="20">
         <v>3.4</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="D17" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="8">
         <v>0.5</v>
@@ -956,47 +959,47 @@
     </row>
     <row r="20" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
         <v>4.3</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="20">
+      <c r="D21" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="20">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C22" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="D22" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>5</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
       </c>
       <c r="D23" s="8">
         <v>0.5</v>
@@ -1004,40 +1007,36 @@
     </row>
     <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
         <v>5.2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="20">
+      <c r="D25" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="20">
         <v>5.3</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
-        <v>6</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="17"/>
       <c r="D26" s="19">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="17"/>
@@ -1045,10 +1044,10 @@
     </row>
     <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="19">
@@ -1059,45 +1058,45 @@
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
-        <v>8</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="17"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="18">
+        <v>6.1</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D28" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="17"/>
@@ -1105,10 +1104,10 @@
     </row>
     <row r="31" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="19">
@@ -1120,10 +1119,10 @@
     </row>
     <row r="32" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="19">
@@ -1134,33 +1133,63 @@
       <c r="G32" s="18"/>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="17">
+        <v>11</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="19">
+        <v>1</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>12</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="19">
+        <v>1</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>13</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D35" s="8">
         <v>8</v>
       </c>
-      <c r="F33" s="16">
-        <f>D34+E3</f>
+      <c r="F35" s="16">
+        <f>D36+E3</f>
         <v>45141.5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11" t="s">
+    <row r="36" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="12">
-        <f>SUM(D3:D33)</f>
+      <c r="D36" s="12">
+        <f>SUM(D3:D35)</f>
         <v>31.5</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="10"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SLR section: Add refs and 1 liners on related work on benchmarks
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85783BB0-5ED3-4746-A0E7-8A76705BC772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1366FE6F-5655-4CBD-8D23-49F4A367277B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -160,6 +171,9 @@
   </si>
   <si>
     <t>Shifted End</t>
+  </si>
+  <si>
+    <t>Literature reserch</t>
   </si>
 </sst>
 </file>
@@ -277,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -353,6 +367,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,11 +713,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,8 +775,8 @@
         <v>44</v>
       </c>
       <c r="I2" s="25">
-        <f ca="1">TODAY()+D36</f>
-        <v>45147.5</v>
+        <f ca="1">TODAY()+D37</f>
+        <v>45148.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -840,70 +865,72 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="30"/>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="34">
+        <v>45117</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="D11" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
         <v>2.1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20">
+      <c r="D12" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D13" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>3.1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="8">
         <v>0.5</v>
@@ -911,58 +938,58 @@
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
         <v>3.3</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="20">
+      <c r="D17" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="20">
         <v>3.4</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="D18" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D19" s="8">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="8">
         <v>0.5</v>
@@ -970,47 +997,47 @@
     </row>
     <row r="21" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
         <v>4.3</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="20">
+      <c r="D22" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="20">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="D23" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>5</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C24" t="s">
-        <v>31</v>
       </c>
       <c r="D24" s="8">
         <v>0.5</v>
@@ -1018,70 +1045,66 @@
     </row>
     <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
         <v>5.2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="20">
+      <c r="D26" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="20">
         <v>5.3</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <v>6</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="17"/>
       <c r="D27" s="19">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18">
-        <v>6.1</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>41</v>
-      </c>
+      <c r="A28" s="17">
+        <v>6</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="17"/>
       <c r="D28" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
-        <v>7</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="17"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18">
+        <v>6.1</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="D29" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="17"/>
@@ -1089,10 +1112,10 @@
     </row>
     <row r="30" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="19">
@@ -1102,16 +1125,16 @@
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
     </row>
-    <row r="31" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="17"/>
@@ -1119,10 +1142,10 @@
     </row>
     <row r="32" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="19">
@@ -1134,10 +1157,10 @@
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="19">
@@ -1149,10 +1172,10 @@
     </row>
     <row r="34" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="19">
@@ -1163,33 +1186,48 @@
       <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="17">
+        <v>12</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="19">
+        <v>1</v>
+      </c>
+      <c r="E35" s="21"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>13</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D36" s="8">
         <v>8</v>
       </c>
-      <c r="F35" s="16">
-        <f>D36+E3</f>
+      <c r="F36" s="16">
+        <f>D37+E3</f>
         <v>45141.5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="11" t="s">
+    <row r="37" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="12">
-        <f>SUM(D3:D35)</f>
+      <c r="D37" s="12">
+        <f>SUM(D3:D36)</f>
         <v>31.5</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="10"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Article - Complete Intro and SLR (related work) sections
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040A94F7-858F-4ACE-A3F3-796759D78CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41FC8C7-143C-4389-8B52-907105E26656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -274,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +358,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +395,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,9 +571,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -571,12 +582,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -627,14 +632,21 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,8 +985,8 @@
   <dimension ref="B1:M42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,9 +997,9 @@
     <col min="4" max="4" width="3.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="41.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="48" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="19.5" x14ac:dyDescent="0.25">
@@ -995,78 +1007,80 @@
         <v>24</v>
       </c>
       <c r="D1" s="15"/>
-      <c r="F1" s="66"/>
+      <c r="F1" s="62"/>
       <c r="G1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="57">
+      <c r="H1" s="54">
         <f>SUM(M4:M42)</f>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>51</v>
       </c>
       <c r="J1" s="28">
-        <v>45162</v>
+        <v>45199</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="53">
+      <c r="L1" s="50">
         <f ca="1">TODAY()</f>
-        <v>45117</v>
-      </c>
-      <c r="M1" s="58"/>
+        <v>45118</v>
+      </c>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="2:13" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
-      <c r="F2" s="66"/>
+      <c r="F2" s="62"/>
       <c r="G2" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="54">
         <f>SUM($G$4:$G$42)</f>
-        <v>44</v>
-      </c>
-      <c r="I2" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="65">
-        <f ca="1">H2+$L$1</f>
-        <v>45161</v>
+      <c r="J2" s="67">
+        <f ca="1">L1+H2+5</f>
+        <v>45171</v>
       </c>
       <c r="K2" s="27"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="58"/>
-    </row>
-    <row r="3" spans="2:13" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="55"/>
+    </row>
+    <row r="3" spans="2:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="50" t="s">
+      <c r="C3" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="59" t="s">
+      <c r="M3" s="56" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1078,7 +1092,7 @@
       <c r="D4" s="36"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
-      <c r="G4" s="43">
+      <c r="G4" s="65">
         <v>0</v>
       </c>
       <c r="H4" s="32">
@@ -1093,8 +1107,8 @@
       <c r="K4" s="33">
         <v>45115</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="60">
+      <c r="L4" s="31"/>
+      <c r="M4" s="57">
         <v>1</v>
       </c>
     </row>
@@ -1108,7 +1122,7 @@
       <c r="D5" s="36"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
-      <c r="G5" s="43">
+      <c r="G5" s="65">
         <v>0</v>
       </c>
       <c r="H5" s="32">
@@ -1121,10 +1135,10 @@
         <v>45111</v>
       </c>
       <c r="K5" s="33">
-        <v>45115</v>
-      </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="60">
+        <v>45118</v>
+      </c>
+      <c r="L5" s="31"/>
+      <c r="M5" s="57">
         <v>2</v>
       </c>
     </row>
@@ -1138,13 +1152,13 @@
       <c r="D6" s="36"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
-      <c r="G6" s="44"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
       <c r="L6" s="31"/>
-      <c r="M6" s="61"/>
+      <c r="M6" s="58"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
@@ -1154,23 +1168,23 @@
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
-      <c r="G7" s="44">
+      <c r="G7" s="66">
         <v>0</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="49">
         <v>45117</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="49">
         <v>45117</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="49">
         <v>45117</v>
       </c>
-      <c r="K7" s="52">
+      <c r="K7" s="49">
         <v>45117</v>
       </c>
       <c r="L7" s="31"/>
-      <c r="M7" s="61">
+      <c r="M7" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1182,15 +1196,24 @@
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
-      <c r="G8" s="44">
-        <v>2</v>
-      </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="G8" s="66">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49">
+        <v>45118</v>
+      </c>
+      <c r="I8" s="49">
+        <f>H8+G8</f>
+        <v>45118</v>
+      </c>
+      <c r="J8" s="49">
+        <v>45117</v>
+      </c>
+      <c r="K8" s="49">
+        <v>45118</v>
+      </c>
       <c r="L8" s="31"/>
-      <c r="M8" s="61">
+      <c r="M8" s="58">
         <v>2</v>
       </c>
     </row>
@@ -1204,13 +1227,13 @@
       <c r="D9" s="36"/>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
-      <c r="G9" s="44"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
       <c r="L9" s="31"/>
-      <c r="M9" s="61"/>
+      <c r="M9" s="58"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="34"/>
@@ -1222,55 +1245,73 @@
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="44">
-        <v>1</v>
-      </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
+      <c r="G10" s="41">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49">
+        <f>K8+1</f>
+        <v>45119</v>
+      </c>
+      <c r="I10" s="49">
+        <f>H10+G10</f>
+        <v>45120</v>
+      </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
       <c r="L10" s="31"/>
-      <c r="M10" s="61">
+      <c r="M10" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="34"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="52" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
-      <c r="G11" s="44">
-        <v>1</v>
-      </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
+      <c r="G11" s="41">
+        <v>1</v>
+      </c>
+      <c r="H11" s="49">
+        <f>I10+1</f>
+        <v>45121</v>
+      </c>
+      <c r="I11" s="49">
+        <f>H11+G11</f>
+        <v>45122</v>
+      </c>
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
       <c r="L11" s="31"/>
-      <c r="M11" s="61">
+      <c r="M11" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="34"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="52" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
-      <c r="G12" s="44">
+      <c r="G12" s="41">
         <v>3</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
+      <c r="H12" s="49">
+        <f>I11+1</f>
+        <v>45123</v>
+      </c>
+      <c r="I12" s="49">
+        <f>H12+G12</f>
+        <v>45126</v>
+      </c>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
       <c r="L12" s="31"/>
-      <c r="M12" s="61">
+      <c r="M12" s="58">
         <v>3</v>
       </c>
     </row>
@@ -1284,15 +1325,21 @@
       </c>
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
-      <c r="G13" s="44">
+      <c r="G13" s="41">
         <v>2</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
+      <c r="H13" s="49">
+        <f t="shared" ref="H13:H42" si="0">I12+1</f>
+        <v>45127</v>
+      </c>
+      <c r="I13" s="49">
+        <f t="shared" ref="I13:I20" si="1">H13+G13</f>
+        <v>45129</v>
+      </c>
       <c r="J13" s="30"/>
       <c r="K13" s="30"/>
       <c r="L13" s="31"/>
-      <c r="M13" s="61">
+      <c r="M13" s="58">
         <v>2</v>
       </c>
     </row>
@@ -1304,15 +1351,21 @@
         <v>3</v>
       </c>
       <c r="F14" s="31"/>
-      <c r="G14" s="44">
-        <v>1</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
+      <c r="G14" s="41">
+        <v>1</v>
+      </c>
+      <c r="H14" s="49">
+        <f t="shared" si="0"/>
+        <v>45130</v>
+      </c>
+      <c r="I14" s="49">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
       <c r="J14" s="30"/>
       <c r="K14" s="30"/>
       <c r="L14" s="31"/>
-      <c r="M14" s="61">
+      <c r="M14" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1320,19 +1373,25 @@
       <c r="B15" s="34"/>
       <c r="C15" s="18"/>
       <c r="D15" s="31"/>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="56"/>
-      <c r="G15" s="44">
-        <v>1</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="41">
+        <v>1</v>
+      </c>
+      <c r="H15" s="49">
+        <f t="shared" si="0"/>
+        <v>45132</v>
+      </c>
+      <c r="I15" s="49">
+        <f t="shared" si="1"/>
+        <v>45133</v>
+      </c>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="31"/>
-      <c r="M15" s="61">
+      <c r="M15" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1340,19 +1399,25 @@
       <c r="B16" s="34"/>
       <c r="C16" s="18"/>
       <c r="D16" s="31"/>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="44">
-        <v>1</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="41">
+        <v>1</v>
+      </c>
+      <c r="H16" s="49">
+        <f t="shared" si="0"/>
+        <v>45134</v>
+      </c>
+      <c r="I16" s="49">
+        <f t="shared" si="1"/>
+        <v>45135</v>
+      </c>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
       <c r="L16" s="31"/>
-      <c r="M16" s="61">
+      <c r="M16" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1364,15 +1429,21 @@
         <v>1</v>
       </c>
       <c r="F17" s="31"/>
-      <c r="G17" s="44">
-        <v>1</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="G17" s="41">
+        <v>1</v>
+      </c>
+      <c r="H17" s="49">
+        <f t="shared" si="0"/>
+        <v>45136</v>
+      </c>
+      <c r="I17" s="49">
+        <f t="shared" si="1"/>
+        <v>45137</v>
+      </c>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="31"/>
-      <c r="M17" s="61">
+      <c r="M17" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1380,19 +1451,25 @@
       <c r="B18" s="34"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="44">
-        <v>1</v>
-      </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="41">
+        <v>1</v>
+      </c>
+      <c r="H18" s="49">
+        <f t="shared" si="0"/>
+        <v>45138</v>
+      </c>
+      <c r="I18" s="49">
+        <f t="shared" si="1"/>
+        <v>45139</v>
+      </c>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="31"/>
-      <c r="M18" s="61">
+      <c r="M18" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1400,19 +1477,25 @@
       <c r="B19" s="34"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="44">
-        <v>1</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="41">
+        <v>1</v>
+      </c>
+      <c r="H19" s="49">
+        <f t="shared" si="0"/>
+        <v>45140</v>
+      </c>
+      <c r="I19" s="49">
+        <f t="shared" si="1"/>
+        <v>45141</v>
+      </c>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="31"/>
-      <c r="M19" s="61">
+      <c r="M19" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1420,19 +1503,25 @@
       <c r="B20" s="34"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="44">
-        <v>1</v>
-      </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="41">
+        <v>1</v>
+      </c>
+      <c r="H20" s="49">
+        <f t="shared" si="0"/>
+        <v>45142</v>
+      </c>
+      <c r="I20" s="49">
+        <f t="shared" si="1"/>
+        <v>45143</v>
+      </c>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
       <c r="L20" s="31"/>
-      <c r="M20" s="61">
+      <c r="M20" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1440,83 +1529,129 @@
       <c r="B21" s="34"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="41">
+        <v>1</v>
+      </c>
+      <c r="H21" s="49">
+        <f t="shared" si="0"/>
+        <v>45144</v>
+      </c>
+      <c r="I21" s="49">
+        <f t="shared" ref="I21:I26" si="2">H21+G21</f>
+        <v>45145</v>
+      </c>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="31"/>
-      <c r="M21" s="61"/>
+      <c r="M21" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="34"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="41">
+        <v>1</v>
+      </c>
+      <c r="H22" s="49">
+        <f t="shared" si="0"/>
+        <v>45146</v>
+      </c>
+      <c r="I22" s="49">
+        <f t="shared" si="2"/>
+        <v>45147</v>
+      </c>
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="31"/>
-      <c r="M22" s="61"/>
+      <c r="M22" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="34"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="41">
+        <v>1</v>
+      </c>
+      <c r="H23" s="49">
+        <f t="shared" si="0"/>
+        <v>45148</v>
+      </c>
+      <c r="I23" s="49">
+        <f t="shared" si="2"/>
+        <v>45149</v>
+      </c>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="31"/>
-      <c r="M23" s="61"/>
+      <c r="M23" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="34"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="67" t="s">
+      <c r="E24" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="41">
+        <v>1</v>
+      </c>
+      <c r="H24" s="49">
+        <f t="shared" si="0"/>
+        <v>45150</v>
+      </c>
+      <c r="I24" s="49">
+        <f t="shared" si="2"/>
+        <v>45151</v>
+      </c>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="31"/>
-      <c r="M24" s="61"/>
+      <c r="M24" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="34"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="56"/>
-      <c r="G25" s="44">
-        <v>1</v>
-      </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="41">
+        <v>1</v>
+      </c>
+      <c r="H25" s="49">
+        <f t="shared" si="0"/>
+        <v>45152</v>
+      </c>
+      <c r="I25" s="49">
+        <f t="shared" si="2"/>
+        <v>45153</v>
+      </c>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="31"/>
-      <c r="M25" s="61">
+      <c r="M25" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1527,16 +1662,22 @@
       <c r="E26" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="56"/>
-      <c r="G26" s="44">
-        <v>1</v>
-      </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="41">
+        <v>1</v>
+      </c>
+      <c r="H26" s="49">
+        <f t="shared" si="0"/>
+        <v>45154</v>
+      </c>
+      <c r="I26" s="49">
+        <f t="shared" si="2"/>
+        <v>45155</v>
+      </c>
       <c r="J26" s="30"/>
       <c r="K26" s="30"/>
       <c r="L26" s="31"/>
-      <c r="M26" s="61">
+      <c r="M26" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1550,15 +1691,21 @@
       <c r="D27" s="36"/>
       <c r="E27" s="31"/>
       <c r="F27" s="31"/>
-      <c r="G27" s="44">
+      <c r="G27" s="41">
         <v>2</v>
       </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
+      <c r="H27" s="49">
+        <f t="shared" si="0"/>
+        <v>45156</v>
+      </c>
+      <c r="I27" s="49">
+        <f t="shared" ref="I27:I29" si="3">H27+G27</f>
+        <v>45158</v>
+      </c>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="31"/>
-      <c r="M27" s="61">
+      <c r="M27" s="58">
         <v>2</v>
       </c>
     </row>
@@ -1570,17 +1717,23 @@
       <c r="D28" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="44">
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="41">
         <v>2</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
+      <c r="H28" s="49">
+        <f t="shared" si="0"/>
+        <v>45159</v>
+      </c>
+      <c r="I28" s="49">
+        <f t="shared" si="3"/>
+        <v>45161</v>
+      </c>
       <c r="J28" s="30"/>
       <c r="K28" s="30"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="61">
+      <c r="L28" s="31"/>
+      <c r="M28" s="58">
         <v>2</v>
       </c>
     </row>
@@ -1592,17 +1745,23 @@
       <c r="D29" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="44">
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="41">
         <v>2</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="49">
+        <f t="shared" si="0"/>
+        <v>45162</v>
+      </c>
+      <c r="I29" s="49">
+        <f t="shared" si="3"/>
+        <v>45164</v>
+      </c>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="61">
+      <c r="L29" s="31"/>
+      <c r="M29" s="58">
         <v>2</v>
       </c>
     </row>
@@ -1610,53 +1769,79 @@
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
       <c r="D30" s="36"/>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="47"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="41">
+        <v>1</v>
+      </c>
+      <c r="H30" s="49">
+        <f t="shared" si="0"/>
+        <v>45165</v>
+      </c>
+      <c r="I30" s="49">
+        <f t="shared" ref="I30:I42" si="4">H30+G30</f>
+        <v>45166</v>
+      </c>
       <c r="J30" s="30"/>
       <c r="K30" s="30"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="61"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
       <c r="D31" s="36"/>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="47"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="41">
+        <v>1</v>
+      </c>
+      <c r="H31" s="49">
+        <f t="shared" si="0"/>
+        <v>45167</v>
+      </c>
+      <c r="I31" s="49">
+        <f t="shared" si="4"/>
+        <v>45168</v>
+      </c>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="61"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="31"/>
       <c r="C32" s="31">
         <v>4.5</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="44">
-        <v>1</v>
-      </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="41">
+        <v>1</v>
+      </c>
+      <c r="H32" s="49">
+        <f t="shared" si="0"/>
+        <v>45169</v>
+      </c>
+      <c r="I32" s="49">
+        <f t="shared" si="4"/>
+        <v>45170</v>
+      </c>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="61">
+      <c r="L32" s="31"/>
+      <c r="M32" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1664,19 +1849,25 @@
       <c r="B33" s="31"/>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="47"/>
-      <c r="G33" s="44">
-        <v>1</v>
-      </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="41">
+        <v>1</v>
+      </c>
+      <c r="H33" s="49">
+        <f t="shared" si="0"/>
+        <v>45171</v>
+      </c>
+      <c r="I33" s="49">
+        <f t="shared" si="4"/>
+        <v>45172</v>
+      </c>
       <c r="J33" s="30"/>
       <c r="K33" s="30"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="61">
+      <c r="L33" s="31"/>
+      <c r="M33" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1684,19 +1875,25 @@
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
       <c r="D34" s="31"/>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="47"/>
-      <c r="G34" s="44">
+      <c r="F34" s="44"/>
+      <c r="G34" s="41">
         <v>0.5</v>
       </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
+      <c r="H34" s="49">
+        <f t="shared" si="0"/>
+        <v>45173</v>
+      </c>
+      <c r="I34" s="49">
+        <f t="shared" si="4"/>
+        <v>45173.5</v>
+      </c>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="61">
+      <c r="L34" s="31"/>
+      <c r="M34" s="58">
         <v>0.5</v>
       </c>
     </row>
@@ -1707,16 +1904,22 @@
       <c r="E35" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="44">
+      <c r="F35" s="44"/>
+      <c r="G35" s="41">
         <v>0.5</v>
       </c>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
+      <c r="H35" s="49">
+        <f t="shared" si="0"/>
+        <v>45174.5</v>
+      </c>
+      <c r="I35" s="49">
+        <f t="shared" si="4"/>
+        <v>45175</v>
+      </c>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="61">
+      <c r="L35" s="31"/>
+      <c r="M35" s="58">
         <v>0.5</v>
       </c>
     </row>
@@ -1729,16 +1932,22 @@
       </c>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="44">
+      <c r="F36" s="44"/>
+      <c r="G36" s="41">
         <v>4</v>
       </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
+      <c r="H36" s="49">
+        <f t="shared" si="0"/>
+        <v>45176</v>
+      </c>
+      <c r="I36" s="49">
+        <f t="shared" si="4"/>
+        <v>45180</v>
+      </c>
       <c r="J36" s="30"/>
       <c r="K36" s="30"/>
       <c r="L36" s="31"/>
-      <c r="M36" s="61">
+      <c r="M36" s="58">
         <v>4</v>
       </c>
     </row>
@@ -1746,61 +1955,79 @@
       <c r="B37" s="34">
         <v>6</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="44">
+      <c r="F37" s="44"/>
+      <c r="G37" s="41">
         <v>2</v>
       </c>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
+      <c r="H37" s="49">
+        <f t="shared" si="0"/>
+        <v>45181</v>
+      </c>
+      <c r="I37" s="49">
+        <f t="shared" si="4"/>
+        <v>45183</v>
+      </c>
       <c r="J37" s="30"/>
       <c r="K37" s="30"/>
       <c r="L37" s="31"/>
-      <c r="M37" s="61">
+      <c r="M37" s="58">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="34"/>
-      <c r="C38" s="49"/>
+      <c r="C38" s="46"/>
       <c r="D38" s="18" t="s">
         <v>55</v>
       </c>
       <c r="E38" s="18"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="44">
-        <v>1</v>
-      </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="41">
+        <v>1</v>
+      </c>
+      <c r="H38" s="49">
+        <f t="shared" si="0"/>
+        <v>45184</v>
+      </c>
+      <c r="I38" s="49">
+        <f t="shared" si="4"/>
+        <v>45185</v>
+      </c>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
       <c r="L38" s="31"/>
-      <c r="M38" s="61">
+      <c r="M38" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="34"/>
-      <c r="C39" s="49"/>
+      <c r="C39" s="46"/>
       <c r="D39" s="18" t="s">
         <v>56</v>
       </c>
       <c r="E39" s="18"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="44">
-        <v>1</v>
-      </c>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="41">
+        <v>1</v>
+      </c>
+      <c r="H39" s="49">
+        <f t="shared" si="0"/>
+        <v>45186</v>
+      </c>
+      <c r="I39" s="49">
+        <f t="shared" si="4"/>
+        <v>45187</v>
+      </c>
       <c r="J39" s="30"/>
       <c r="K39" s="30"/>
       <c r="L39" s="31"/>
-      <c r="M39" s="61">
+      <c r="M39" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1811,16 +2038,22 @@
         <v>41</v>
       </c>
       <c r="E40" s="18"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="44">
-        <v>1</v>
-      </c>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="41">
+        <v>1</v>
+      </c>
+      <c r="H40" s="49">
+        <f t="shared" si="0"/>
+        <v>45188</v>
+      </c>
+      <c r="I40" s="49">
+        <f t="shared" si="4"/>
+        <v>45189</v>
+      </c>
       <c r="J40" s="30"/>
       <c r="K40" s="30"/>
       <c r="L40" s="31"/>
-      <c r="M40" s="61">
+      <c r="M40" s="58">
         <v>1</v>
       </c>
     </row>
@@ -1828,43 +2061,55 @@
       <c r="B41" s="34">
         <v>7</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="46" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="44">
+      <c r="F41" s="44"/>
+      <c r="G41" s="41">
         <v>3</v>
       </c>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
+      <c r="H41" s="49">
+        <f t="shared" si="0"/>
+        <v>45190</v>
+      </c>
+      <c r="I41" s="49">
+        <f t="shared" si="4"/>
+        <v>45193</v>
+      </c>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
       <c r="L41" s="31"/>
-      <c r="M41" s="61">
+      <c r="M41" s="58">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="39">
+      <c r="B42" s="38">
         <v>8</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="45">
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="42">
         <v>5</v>
       </c>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
+      <c r="H42" s="49">
+        <f t="shared" si="0"/>
+        <v>45194</v>
+      </c>
+      <c r="I42" s="49">
+        <f t="shared" si="4"/>
+        <v>45199</v>
+      </c>
       <c r="J42" s="35"/>
       <c r="K42" s="35"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="62">
+      <c r="L42" s="37"/>
+      <c r="M42" s="59">
         <v>5</v>
       </c>
     </row>
@@ -1939,7 +2184,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">TODAY()+D37</f>
-        <v>45148.5</v>
+        <v>45149.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Article -- begin A2C
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41FC8C7-143C-4389-8B52-907105E26656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5A48DB-E4B3-4A35-92FE-56DF13FBA6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -265,6 +254,9 @@
   </si>
   <si>
     <t>Transition Function</t>
+  </si>
+  <si>
+    <t>RL note</t>
   </si>
 </sst>
 </file>
@@ -367,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -648,6 +646,12 @@
     <xf numFmtId="16" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,11 +986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B960D0FC-F9A3-469E-ABD5-093C4BA06CC0}">
-  <dimension ref="B1:M42"/>
+  <dimension ref="B1:M43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,21 +1016,21 @@
         <v>67</v>
       </c>
       <c r="H1" s="54">
-        <f>SUM(M4:M42)</f>
-        <v>54</v>
+        <f>SUM(M4:M43)</f>
+        <v>55</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>51</v>
       </c>
       <c r="J1" s="28">
-        <v>45199</v>
+        <v>45184</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>61</v>
       </c>
       <c r="L1" s="50">
         <f ca="1">TODAY()</f>
-        <v>45118</v>
+        <v>45120</v>
       </c>
       <c r="M1" s="55"/>
     </row>
@@ -1038,15 +1042,15 @@
         <v>68</v>
       </c>
       <c r="H2" s="54">
-        <f>SUM($G$4:$G$42)</f>
-        <v>48</v>
+        <f>SUM($G$4:$G$43)</f>
+        <v>47</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>70</v>
       </c>
       <c r="J2" s="67">
         <f ca="1">L1+H2+5</f>
-        <v>45171</v>
+        <v>45172</v>
       </c>
       <c r="K2" s="27"/>
       <c r="L2" s="50"/>
@@ -1245,8 +1249,8 @@
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="41">
-        <v>1</v>
+      <c r="G10" s="66">
+        <v>0</v>
       </c>
       <c r="H10" s="49">
         <f>K8+1</f>
@@ -1254,10 +1258,14 @@
       </c>
       <c r="I10" s="49">
         <f>H10+G10</f>
-        <v>45120</v>
-      </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
+        <v>45119</v>
+      </c>
+      <c r="J10" s="49">
+        <v>45119</v>
+      </c>
+      <c r="K10" s="49">
+        <v>45119</v>
+      </c>
       <c r="L10" s="31"/>
       <c r="M10" s="58">
         <v>1</v>
@@ -1267,23 +1275,27 @@
       <c r="B11" s="34"/>
       <c r="C11" s="18"/>
       <c r="D11" s="52" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
-      <c r="G11" s="41">
-        <v>1</v>
+      <c r="G11" s="66">
+        <v>0</v>
       </c>
       <c r="H11" s="49">
         <f>I10+1</f>
-        <v>45121</v>
+        <v>45120</v>
       </c>
       <c r="I11" s="49">
         <f>H11+G11</f>
-        <v>45122</v>
-      </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+        <v>45120</v>
+      </c>
+      <c r="J11" s="49">
+        <v>45119</v>
+      </c>
+      <c r="K11" s="49">
+        <v>45119</v>
+      </c>
       <c r="L11" s="31"/>
       <c r="M11" s="58">
         <v>1</v>
@@ -1293,100 +1305,102 @@
       <c r="B12" s="34"/>
       <c r="C12" s="18"/>
       <c r="D12" s="52" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" s="49">
         <f>I11+1</f>
-        <v>45123</v>
+        <v>45121</v>
       </c>
       <c r="I12" s="49">
         <f>H12+G12</f>
-        <v>45126</v>
+        <v>45122</v>
       </c>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
       <c r="L12" s="31"/>
       <c r="M12" s="58">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
-      <c r="C13" s="18">
-        <v>3.2</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="41">
-        <v>2</v>
-      </c>
-      <c r="H13" s="49">
-        <f t="shared" ref="H13:H42" si="0">I12+1</f>
-        <v>45127</v>
-      </c>
-      <c r="I13" s="49">
-        <f t="shared" ref="I13:I20" si="1">H13+G13</f>
-        <v>45129</v>
-      </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69">
+        <v>3</v>
+      </c>
+      <c r="H13" s="70">
+        <f>I12+1</f>
+        <v>45123</v>
+      </c>
+      <c r="I13" s="70">
+        <f>H13+G13</f>
+        <v>45126</v>
+      </c>
+      <c r="J13" s="70">
+        <v>45120</v>
+      </c>
+      <c r="K13" s="71"/>
       <c r="L13" s="31"/>
       <c r="M13" s="58">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="34"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="31" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="18">
+        <v>3.2</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="49">
-        <f t="shared" si="0"/>
-        <v>45130</v>
+        <f t="shared" ref="H14:H43" si="0">I13+1</f>
+        <v>45127</v>
       </c>
       <c r="I14" s="49">
-        <f t="shared" si="1"/>
-        <v>45131</v>
+        <f t="shared" ref="I14:I21" si="1">H14+G14</f>
+        <v>45129</v>
       </c>
       <c r="J14" s="30"/>
       <c r="K14" s="30"/>
       <c r="L14" s="31"/>
       <c r="M14" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
       <c r="C15" s="18"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="53"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="31"/>
       <c r="G15" s="41">
         <v>1</v>
       </c>
       <c r="H15" s="49">
         <f t="shared" si="0"/>
-        <v>45132</v>
+        <v>45130</v>
       </c>
       <c r="I15" s="49">
         <f t="shared" si="1"/>
-        <v>45133</v>
+        <v>45131</v>
       </c>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
@@ -1400,7 +1414,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="31"/>
       <c r="E16" s="53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="53"/>
       <c r="G16" s="41">
@@ -1408,11 +1422,11 @@
       </c>
       <c r="H16" s="49">
         <f t="shared" si="0"/>
-        <v>45134</v>
+        <v>45132</v>
       </c>
       <c r="I16" s="49">
         <f t="shared" si="1"/>
-        <v>45135</v>
+        <v>45133</v>
       </c>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
@@ -1424,21 +1438,21 @@
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="34"/>
       <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="53"/>
       <c r="G17" s="41">
         <v>1</v>
       </c>
       <c r="H17" s="49">
         <f t="shared" si="0"/>
-        <v>45136</v>
+        <v>45134</v>
       </c>
       <c r="I17" s="49">
         <f t="shared" si="1"/>
-        <v>45137</v>
+        <v>45135</v>
       </c>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
@@ -1451,20 +1465,20 @@
       <c r="B18" s="34"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="53"/>
+      <c r="E18" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="31"/>
       <c r="G18" s="41">
         <v>1</v>
       </c>
       <c r="H18" s="49">
         <f t="shared" si="0"/>
-        <v>45138</v>
+        <v>45136</v>
       </c>
       <c r="I18" s="49">
         <f t="shared" si="1"/>
-        <v>45139</v>
+        <v>45137</v>
       </c>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
@@ -1478,7 +1492,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="41">
@@ -1486,11 +1500,11 @@
       </c>
       <c r="H19" s="49">
         <f t="shared" si="0"/>
-        <v>45140</v>
+        <v>45138</v>
       </c>
       <c r="I19" s="49">
         <f t="shared" si="1"/>
-        <v>45141</v>
+        <v>45139</v>
       </c>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
@@ -1504,7 +1518,7 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="53" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="41">
@@ -1512,11 +1526,11 @@
       </c>
       <c r="H20" s="49">
         <f t="shared" si="0"/>
-        <v>45142</v>
+        <v>45140</v>
       </c>
       <c r="I20" s="49">
         <f t="shared" si="1"/>
-        <v>45143</v>
+        <v>45141</v>
       </c>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
@@ -1530,7 +1544,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="53"/>
       <c r="G21" s="41">
@@ -1538,11 +1552,11 @@
       </c>
       <c r="H21" s="49">
         <f t="shared" si="0"/>
-        <v>45144</v>
+        <v>45142</v>
       </c>
       <c r="I21" s="49">
-        <f t="shared" ref="I21:I26" si="2">H21+G21</f>
-        <v>45145</v>
+        <f t="shared" si="1"/>
+        <v>45143</v>
       </c>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
@@ -1556,7 +1570,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="41">
@@ -1564,11 +1578,11 @@
       </c>
       <c r="H22" s="49">
         <f t="shared" si="0"/>
-        <v>45146</v>
+        <v>45144</v>
       </c>
       <c r="I22" s="49">
-        <f t="shared" si="2"/>
-        <v>45147</v>
+        <f t="shared" ref="I22:I27" si="2">H22+G22</f>
+        <v>45145</v>
       </c>
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
@@ -1582,7 +1596,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="53" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="41">
@@ -1590,11 +1604,11 @@
       </c>
       <c r="H23" s="49">
         <f t="shared" si="0"/>
-        <v>45148</v>
+        <v>45146</v>
       </c>
       <c r="I23" s="49">
         <f t="shared" si="2"/>
-        <v>45149</v>
+        <v>45147</v>
       </c>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
@@ -1608,7 +1622,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="41">
@@ -1616,11 +1630,11 @@
       </c>
       <c r="H24" s="49">
         <f t="shared" si="0"/>
-        <v>45150</v>
+        <v>45148</v>
       </c>
       <c r="I24" s="49">
         <f t="shared" si="2"/>
-        <v>45151</v>
+        <v>45149</v>
       </c>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
@@ -1633,8 +1647,8 @@
       <c r="B25" s="34"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="44" t="s">
-        <v>14</v>
+      <c r="E25" s="53" t="s">
+        <v>75</v>
       </c>
       <c r="F25" s="53"/>
       <c r="G25" s="41">
@@ -1642,11 +1656,11 @@
       </c>
       <c r="H25" s="49">
         <f t="shared" si="0"/>
-        <v>45152</v>
+        <v>45150</v>
       </c>
       <c r="I25" s="49">
         <f t="shared" si="2"/>
-        <v>45153</v>
+        <v>45151</v>
       </c>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
@@ -1659,8 +1673,8 @@
       <c r="B26" s="34"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="18" t="s">
-        <v>15</v>
+      <c r="E26" s="44" t="s">
+        <v>14</v>
       </c>
       <c r="F26" s="53"/>
       <c r="G26" s="41">
@@ -1668,11 +1682,11 @@
       </c>
       <c r="H26" s="49">
         <f t="shared" si="0"/>
-        <v>45154</v>
+        <v>45152</v>
       </c>
       <c r="I26" s="49">
         <f t="shared" si="2"/>
-        <v>45155</v>
+        <v>45153</v>
       </c>
       <c r="J26" s="30"/>
       <c r="K26" s="30"/>
@@ -1682,53 +1696,51 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="34">
-        <v>4</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="53"/>
       <c r="G27" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="49">
         <f t="shared" si="0"/>
-        <v>45156</v>
+        <v>45154</v>
       </c>
       <c r="I27" s="49">
-        <f t="shared" ref="I27:I29" si="3">H27+G27</f>
-        <v>45158</v>
+        <f t="shared" si="2"/>
+        <v>45155</v>
       </c>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="31"/>
       <c r="M27" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="31"/>
-      <c r="C28" s="31">
-        <v>4.3</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
+      <c r="B28" s="34">
+        <v>4</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="36"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="41">
         <v>2</v>
       </c>
       <c r="H28" s="49">
         <f t="shared" si="0"/>
-        <v>45159</v>
+        <v>45156</v>
       </c>
       <c r="I28" s="49">
-        <f t="shared" si="3"/>
-        <v>45161</v>
+        <f t="shared" ref="I28:I30" si="3">H28+G28</f>
+        <v>45158</v>
       </c>
       <c r="J28" s="30"/>
       <c r="K28" s="30"/>
@@ -1740,10 +1752,10 @@
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="31"/>
       <c r="C29" s="31">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
@@ -1752,11 +1764,11 @@
       </c>
       <c r="H29" s="49">
         <f t="shared" si="0"/>
-        <v>45162</v>
+        <v>45159</v>
       </c>
       <c r="I29" s="49">
         <f t="shared" si="3"/>
-        <v>45164</v>
+        <v>45161</v>
       </c>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
@@ -1767,28 +1779,30 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="C30" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="44"/>
       <c r="F30" s="44"/>
       <c r="G30" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="49">
         <f t="shared" si="0"/>
-        <v>45165</v>
+        <v>45162</v>
       </c>
       <c r="I30" s="49">
-        <f t="shared" ref="I30:I42" si="4">H30+G30</f>
-        <v>45166</v>
+        <f t="shared" si="3"/>
+        <v>45164</v>
       </c>
       <c r="J30" s="30"/>
       <c r="K30" s="30"/>
       <c r="L30" s="31"/>
       <c r="M30" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
@@ -1796,7 +1810,7 @@
       <c r="C31" s="31"/>
       <c r="D31" s="36"/>
       <c r="E31" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" s="44"/>
       <c r="G31" s="41">
@@ -1804,11 +1818,11 @@
       </c>
       <c r="H31" s="49">
         <f t="shared" si="0"/>
-        <v>45167</v>
+        <v>45165</v>
       </c>
       <c r="I31" s="49">
-        <f t="shared" si="4"/>
-        <v>45168</v>
+        <f t="shared" ref="I31:I43" si="4">H31+G31</f>
+        <v>45166</v>
       </c>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
@@ -1819,24 +1833,22 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="31"/>
-      <c r="C32" s="31">
-        <v>4.5</v>
-      </c>
-      <c r="D32" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="44"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="44" t="s">
+        <v>66</v>
+      </c>
       <c r="F32" s="44"/>
       <c r="G32" s="41">
         <v>1</v>
       </c>
       <c r="H32" s="49">
         <f t="shared" si="0"/>
-        <v>45169</v>
+        <v>45167</v>
       </c>
       <c r="I32" s="49">
         <f t="shared" si="4"/>
-        <v>45170</v>
+        <v>45168</v>
       </c>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
@@ -1847,22 +1859,24 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="44" t="s">
-        <v>11</v>
-      </c>
+      <c r="C33" s="31">
+        <v>4.5</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="44"/>
       <c r="F33" s="44"/>
       <c r="G33" s="41">
         <v>1</v>
       </c>
       <c r="H33" s="49">
         <f t="shared" si="0"/>
-        <v>45171</v>
+        <v>45169</v>
       </c>
       <c r="I33" s="49">
         <f t="shared" si="4"/>
-        <v>45172</v>
+        <v>45170</v>
       </c>
       <c r="J33" s="30"/>
       <c r="K33" s="30"/>
@@ -1876,33 +1890,33 @@
       <c r="C34" s="31"/>
       <c r="D34" s="31"/>
       <c r="E34" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="41">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H34" s="49">
         <f t="shared" si="0"/>
-        <v>45173</v>
+        <v>45171</v>
       </c>
       <c r="I34" s="49">
         <f t="shared" si="4"/>
-        <v>45173.5</v>
+        <v>45172</v>
       </c>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
       <c r="L34" s="31"/>
       <c r="M34" s="58">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
-      <c r="E35" s="31" t="s">
-        <v>13</v>
+      <c r="E35" s="44" t="s">
+        <v>12</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="41">
@@ -1910,11 +1924,11 @@
       </c>
       <c r="H35" s="49">
         <f t="shared" si="0"/>
-        <v>45174.5</v>
+        <v>45173</v>
       </c>
       <c r="I35" s="49">
         <f t="shared" si="4"/>
-        <v>45175</v>
+        <v>45173.5</v>
       </c>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
@@ -1924,92 +1938,92 @@
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="34">
-        <v>5</v>
-      </c>
-      <c r="C36" s="36" t="s">
-        <v>54</v>
-      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
+      <c r="E36" s="31" t="s">
+        <v>13</v>
+      </c>
       <c r="F36" s="44"/>
       <c r="G36" s="41">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="H36" s="49">
         <f t="shared" si="0"/>
-        <v>45176</v>
+        <v>45174.5</v>
       </c>
       <c r="I36" s="49">
         <f t="shared" si="4"/>
-        <v>45180</v>
+        <v>45175</v>
       </c>
       <c r="J36" s="30"/>
       <c r="K36" s="30"/>
       <c r="L36" s="31"/>
       <c r="M36" s="58">
-        <v>4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="34">
-        <v>6</v>
-      </c>
-      <c r="C37" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
       <c r="F37" s="44"/>
       <c r="G37" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37" s="49">
         <f t="shared" si="0"/>
-        <v>45181</v>
+        <v>45176</v>
       </c>
       <c r="I37" s="49">
         <f t="shared" si="4"/>
-        <v>45183</v>
+        <v>45180</v>
       </c>
       <c r="J37" s="30"/>
       <c r="K37" s="30"/>
       <c r="L37" s="31"/>
       <c r="M37" s="58">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="18" t="s">
-        <v>55</v>
-      </c>
+      <c r="B38" s="34">
+        <v>6</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="44"/>
       <c r="G38" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38" s="49">
         <f t="shared" si="0"/>
-        <v>45184</v>
+        <v>45181</v>
       </c>
       <c r="I38" s="49">
         <f t="shared" si="4"/>
-        <v>45185</v>
+        <v>45183</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
       <c r="L38" s="31"/>
       <c r="M38" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="34"/>
       <c r="C39" s="46"/>
       <c r="D39" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="44"/>
@@ -2018,11 +2032,11 @@
       </c>
       <c r="H39" s="49">
         <f t="shared" si="0"/>
-        <v>45186</v>
+        <v>45184</v>
       </c>
       <c r="I39" s="49">
         <f t="shared" si="4"/>
-        <v>45187</v>
+        <v>45185</v>
       </c>
       <c r="J39" s="30"/>
       <c r="K39" s="30"/>
@@ -2033,9 +2047,9 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="34"/>
-      <c r="C40" s="18"/>
+      <c r="C40" s="46"/>
       <c r="D40" s="18" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="44"/>
@@ -2044,11 +2058,11 @@
       </c>
       <c r="H40" s="49">
         <f t="shared" si="0"/>
-        <v>45188</v>
+        <v>45186</v>
       </c>
       <c r="I40" s="49">
         <f t="shared" si="4"/>
-        <v>45189</v>
+        <v>45187</v>
       </c>
       <c r="J40" s="30"/>
       <c r="K40" s="30"/>
@@ -2058,58 +2072,84 @@
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="34">
-        <v>7</v>
-      </c>
-      <c r="C41" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="18"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="44"/>
       <c r="G41" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H41" s="49">
         <f t="shared" si="0"/>
-        <v>45190</v>
+        <v>45188</v>
       </c>
       <c r="I41" s="49">
         <f t="shared" si="4"/>
-        <v>45193</v>
+        <v>45189</v>
       </c>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
       <c r="L41" s="31"/>
       <c r="M41" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="34">
+        <v>7</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="38">
-        <v>8</v>
-      </c>
-      <c r="C42" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="42">
-        <v>5</v>
-      </c>
       <c r="H42" s="49">
         <f t="shared" si="0"/>
-        <v>45194</v>
+        <v>45190</v>
       </c>
       <c r="I42" s="49">
         <f t="shared" si="4"/>
+        <v>45193</v>
+      </c>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="38">
+        <v>8</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="42">
+        <v>5</v>
+      </c>
+      <c r="H43" s="49">
+        <f t="shared" si="0"/>
+        <v>45194</v>
+      </c>
+      <c r="I43" s="49">
+        <f t="shared" si="4"/>
         <v>45199</v>
       </c>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="59">
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="59">
         <v>5</v>
       </c>
     </row>
@@ -2184,7 +2224,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">TODAY()+D37</f>
-        <v>45149.5</v>
+        <v>45151.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PPO and REINFORCE updated
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D75DFF3-A15D-4A70-9AC4-D36A6168FF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78333FF-A3EE-4C45-B12D-56BC521EDAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,7 +1001,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,14 +1054,14 @@
       </c>
       <c r="H2" s="54">
         <f>SUM($G$4:$G$43)</f>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>70</v>
       </c>
       <c r="J2" s="67">
         <f ca="1">L1+H2+5</f>
-        <v>45170</v>
+        <v>45168</v>
       </c>
       <c r="K2" s="27"/>
       <c r="L2" s="50"/>
@@ -1268,7 +1268,7 @@
         <v>45119</v>
       </c>
       <c r="I10" s="49">
-        <f>H10+G10</f>
+        <f t="shared" ref="I10:I15" si="0">H10+G10</f>
         <v>45119</v>
       </c>
       <c r="J10" s="49">
@@ -1298,7 +1298,7 @@
         <v>45120</v>
       </c>
       <c r="I11" s="49">
-        <f>H11+G11</f>
+        <f t="shared" si="0"/>
         <v>45120</v>
       </c>
       <c r="J11" s="49">
@@ -1321,15 +1321,15 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="49">
         <f>I11+1</f>
         <v>45121</v>
       </c>
       <c r="I12" s="49">
-        <f>H12+G12</f>
-        <v>45122</v>
+        <f t="shared" si="0"/>
+        <v>45121</v>
       </c>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
@@ -1347,15 +1347,15 @@
       <c r="E13" s="68"/>
       <c r="F13" s="68"/>
       <c r="G13" s="69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="70">
         <f>I12+1</f>
-        <v>45123</v>
+        <v>45122</v>
       </c>
       <c r="I13" s="70">
-        <f>H13+G13</f>
-        <v>45124</v>
+        <f t="shared" si="0"/>
+        <v>45122</v>
       </c>
       <c r="J13" s="70">
         <v>45120</v>
@@ -1367,28 +1367,28 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
-      <c r="C14" s="18">
-        <v>3.2</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>64</v>
-      </c>
+      <c r="B14" s="34">
+        <v>4</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="36"/>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="41">
         <v>2</v>
       </c>
       <c r="H14" s="49">
-        <f t="shared" ref="H14:H43" si="0">I13+1</f>
+        <f>I13+1</f>
+        <v>45123</v>
+      </c>
+      <c r="I14" s="49">
+        <f t="shared" si="0"/>
         <v>45125</v>
       </c>
-      <c r="I14" s="49">
-        <f t="shared" ref="I14:I21" si="1">H14+G14</f>
-        <v>45127</v>
-      </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
       <c r="L14" s="31"/>
       <c r="M14" s="58">
         <v>2</v>
@@ -1396,48 +1396,48 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="31" t="s">
-        <v>3</v>
-      </c>
+      <c r="C15" s="18">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="31"/>
       <c r="F15" s="31"/>
       <c r="G15" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="49">
+        <v>45118</v>
+      </c>
+      <c r="I15" s="49">
         <f t="shared" si="0"/>
-        <v>45128</v>
-      </c>
-      <c r="I15" s="49">
-        <f t="shared" si="1"/>
-        <v>45129</v>
+        <v>45120</v>
       </c>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="31"/>
       <c r="M15" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="53"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="31"/>
       <c r="G16" s="41">
         <v>1</v>
       </c>
       <c r="H16" s="49">
-        <f t="shared" si="0"/>
-        <v>45130</v>
+        <v>45119</v>
       </c>
       <c r="I16" s="49">
-        <f t="shared" si="1"/>
-        <v>45131</v>
+        <f t="shared" ref="I16:I28" si="1">H16+G16</f>
+        <v>45120</v>
       </c>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
@@ -1451,19 +1451,18 @@
       <c r="C17" s="18"/>
       <c r="D17" s="31"/>
       <c r="E17" s="53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="53"/>
       <c r="G17" s="41">
         <v>1</v>
       </c>
       <c r="H17" s="49">
-        <f t="shared" si="0"/>
-        <v>45132</v>
+        <v>45120</v>
       </c>
       <c r="I17" s="49">
         <f t="shared" si="1"/>
-        <v>45133</v>
+        <v>45121</v>
       </c>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
@@ -1475,21 +1474,20 @@
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="34"/>
       <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="53"/>
       <c r="G18" s="41">
         <v>1</v>
       </c>
       <c r="H18" s="49">
-        <f t="shared" si="0"/>
-        <v>45134</v>
+        <v>45121</v>
       </c>
       <c r="I18" s="49">
         <f t="shared" si="1"/>
-        <v>45135</v>
+        <v>45122</v>
       </c>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
@@ -1502,20 +1500,19 @@
       <c r="B19" s="34"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="53"/>
+      <c r="E19" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="31"/>
       <c r="G19" s="41">
         <v>1</v>
       </c>
       <c r="H19" s="49">
-        <f t="shared" si="0"/>
-        <v>45136</v>
+        <v>45122</v>
       </c>
       <c r="I19" s="49">
         <f t="shared" si="1"/>
-        <v>45137</v>
+        <v>45123</v>
       </c>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
@@ -1529,19 +1526,18 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="41">
         <v>1</v>
       </c>
       <c r="H20" s="49">
-        <f t="shared" si="0"/>
-        <v>45138</v>
+        <v>45123</v>
       </c>
       <c r="I20" s="49">
         <f t="shared" si="1"/>
-        <v>45139</v>
+        <v>45124</v>
       </c>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
@@ -1555,19 +1551,18 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="53" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="F21" s="53"/>
       <c r="G21" s="41">
         <v>1</v>
       </c>
       <c r="H21" s="49">
-        <f t="shared" si="0"/>
-        <v>45140</v>
+        <v>45124</v>
       </c>
       <c r="I21" s="49">
         <f t="shared" si="1"/>
-        <v>45141</v>
+        <v>45125</v>
       </c>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
@@ -1581,19 +1576,18 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="41">
         <v>1</v>
       </c>
       <c r="H22" s="49">
-        <f t="shared" si="0"/>
-        <v>45142</v>
+        <v>45125</v>
       </c>
       <c r="I22" s="49">
-        <f t="shared" ref="I22:I27" si="2">H22+G22</f>
-        <v>45143</v>
+        <f t="shared" si="1"/>
+        <v>45126</v>
       </c>
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
@@ -1607,19 +1601,18 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="41">
         <v>1</v>
       </c>
       <c r="H23" s="49">
-        <f t="shared" si="0"/>
-        <v>45144</v>
+        <v>45126</v>
       </c>
       <c r="I23" s="49">
-        <f t="shared" si="2"/>
-        <v>45145</v>
+        <f t="shared" si="1"/>
+        <v>45127</v>
       </c>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
@@ -1633,19 +1626,18 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="53" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="41">
         <v>1</v>
       </c>
       <c r="H24" s="49">
-        <f t="shared" si="0"/>
-        <v>45146</v>
+        <v>45127</v>
       </c>
       <c r="I24" s="49">
-        <f t="shared" si="2"/>
-        <v>45147</v>
+        <f t="shared" si="1"/>
+        <v>45128</v>
       </c>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
@@ -1659,19 +1651,18 @@
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F25" s="53"/>
       <c r="G25" s="41">
         <v>1</v>
       </c>
       <c r="H25" s="49">
-        <f t="shared" si="0"/>
-        <v>45148</v>
+        <v>45128</v>
       </c>
       <c r="I25" s="49">
-        <f t="shared" si="2"/>
-        <v>45149</v>
+        <f t="shared" si="1"/>
+        <v>45129</v>
       </c>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
@@ -1684,20 +1675,19 @@
       <c r="B26" s="34"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="44" t="s">
-        <v>14</v>
+      <c r="E26" s="53" t="s">
+        <v>75</v>
       </c>
       <c r="F26" s="53"/>
       <c r="G26" s="41">
         <v>1</v>
       </c>
       <c r="H26" s="49">
-        <f t="shared" si="0"/>
-        <v>45150</v>
+        <v>45129</v>
       </c>
       <c r="I26" s="49">
-        <f t="shared" si="2"/>
-        <v>45151</v>
+        <f t="shared" si="1"/>
+        <v>45130</v>
       </c>
       <c r="J26" s="30"/>
       <c r="K26" s="30"/>
@@ -1710,20 +1700,19 @@
       <c r="B27" s="34"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="18" t="s">
-        <v>15</v>
+      <c r="E27" s="44" t="s">
+        <v>14</v>
       </c>
       <c r="F27" s="53"/>
       <c r="G27" s="41">
         <v>1</v>
       </c>
       <c r="H27" s="49">
-        <f t="shared" si="0"/>
-        <v>45152</v>
+        <v>45130</v>
       </c>
       <c r="I27" s="49">
-        <f t="shared" si="2"/>
-        <v>45153</v>
+        <f t="shared" si="1"/>
+        <v>45131</v>
       </c>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
@@ -1733,31 +1722,28 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="34">
-        <v>4</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="53"/>
       <c r="G28" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="49">
-        <f t="shared" si="0"/>
-        <v>45154</v>
+        <v>45131</v>
       </c>
       <c r="I28" s="49">
-        <f t="shared" ref="I28:I30" si="3">H28+G28</f>
-        <v>45156</v>
+        <f t="shared" si="1"/>
+        <v>45132</v>
       </c>
       <c r="J28" s="30"/>
       <c r="K28" s="30"/>
       <c r="L28" s="31"/>
       <c r="M28" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
@@ -1774,12 +1760,11 @@
         <v>2</v>
       </c>
       <c r="H29" s="49">
-        <f t="shared" si="0"/>
-        <v>45157</v>
+        <v>45130</v>
       </c>
       <c r="I29" s="49">
-        <f t="shared" si="3"/>
-        <v>45159</v>
+        <f t="shared" ref="I29" si="2">H29+G29</f>
+        <v>45132</v>
       </c>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
@@ -1802,12 +1787,12 @@
         <v>2</v>
       </c>
       <c r="H30" s="49">
-        <f t="shared" si="0"/>
-        <v>45160</v>
+        <f t="shared" ref="H30:H43" si="3">I29+1</f>
+        <v>45133</v>
       </c>
       <c r="I30" s="49">
-        <f t="shared" si="3"/>
-        <v>45162</v>
+        <f t="shared" ref="I30" si="4">H30+G30</f>
+        <v>45135</v>
       </c>
       <c r="J30" s="30"/>
       <c r="K30" s="30"/>
@@ -1828,12 +1813,12 @@
         <v>1</v>
       </c>
       <c r="H31" s="49">
-        <f t="shared" si="0"/>
-        <v>45163</v>
+        <f t="shared" si="3"/>
+        <v>45136</v>
       </c>
       <c r="I31" s="49">
-        <f t="shared" ref="I31:I43" si="4">H31+G31</f>
-        <v>45164</v>
+        <f t="shared" ref="I31:I43" si="5">H31+G31</f>
+        <v>45137</v>
       </c>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
@@ -1854,12 +1839,12 @@
         <v>1</v>
       </c>
       <c r="H32" s="49">
-        <f t="shared" si="0"/>
-        <v>45165</v>
+        <f t="shared" si="3"/>
+        <v>45138</v>
       </c>
       <c r="I32" s="49">
-        <f t="shared" si="4"/>
-        <v>45166</v>
+        <f t="shared" si="5"/>
+        <v>45139</v>
       </c>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
@@ -1882,12 +1867,12 @@
         <v>1</v>
       </c>
       <c r="H33" s="49">
-        <f t="shared" si="0"/>
-        <v>45167</v>
+        <f t="shared" si="3"/>
+        <v>45140</v>
       </c>
       <c r="I33" s="49">
-        <f t="shared" si="4"/>
-        <v>45168</v>
+        <f t="shared" si="5"/>
+        <v>45141</v>
       </c>
       <c r="J33" s="30"/>
       <c r="K33" s="30"/>
@@ -1908,12 +1893,12 @@
         <v>1</v>
       </c>
       <c r="H34" s="49">
-        <f t="shared" si="0"/>
-        <v>45169</v>
+        <f t="shared" si="3"/>
+        <v>45142</v>
       </c>
       <c r="I34" s="49">
-        <f t="shared" si="4"/>
-        <v>45170</v>
+        <f t="shared" si="5"/>
+        <v>45143</v>
       </c>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
@@ -1934,12 +1919,12 @@
         <v>0.5</v>
       </c>
       <c r="H35" s="49">
-        <f t="shared" si="0"/>
-        <v>45171</v>
+        <f t="shared" si="3"/>
+        <v>45144</v>
       </c>
       <c r="I35" s="49">
-        <f t="shared" si="4"/>
-        <v>45171.5</v>
+        <f t="shared" si="5"/>
+        <v>45144.5</v>
       </c>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
@@ -1960,12 +1945,12 @@
         <v>0.5</v>
       </c>
       <c r="H36" s="49">
-        <f t="shared" si="0"/>
-        <v>45172.5</v>
+        <f t="shared" si="3"/>
+        <v>45145.5</v>
       </c>
       <c r="I36" s="49">
-        <f t="shared" si="4"/>
-        <v>45173</v>
+        <f t="shared" si="5"/>
+        <v>45146</v>
       </c>
       <c r="J36" s="30"/>
       <c r="K36" s="30"/>
@@ -1988,12 +1973,12 @@
         <v>4</v>
       </c>
       <c r="H37" s="49">
-        <f t="shared" si="0"/>
-        <v>45174</v>
+        <f t="shared" si="3"/>
+        <v>45147</v>
       </c>
       <c r="I37" s="49">
-        <f t="shared" si="4"/>
-        <v>45178</v>
+        <f t="shared" si="5"/>
+        <v>45151</v>
       </c>
       <c r="J37" s="30"/>
       <c r="K37" s="30"/>
@@ -2016,12 +2001,12 @@
         <v>2</v>
       </c>
       <c r="H38" s="49">
-        <f t="shared" si="0"/>
-        <v>45179</v>
+        <f t="shared" si="3"/>
+        <v>45152</v>
       </c>
       <c r="I38" s="49">
-        <f t="shared" si="4"/>
-        <v>45181</v>
+        <f t="shared" si="5"/>
+        <v>45154</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
@@ -2042,12 +2027,12 @@
         <v>1</v>
       </c>
       <c r="H39" s="49">
-        <f t="shared" si="0"/>
-        <v>45182</v>
+        <f t="shared" si="3"/>
+        <v>45155</v>
       </c>
       <c r="I39" s="49">
-        <f t="shared" si="4"/>
-        <v>45183</v>
+        <f t="shared" si="5"/>
+        <v>45156</v>
       </c>
       <c r="J39" s="30"/>
       <c r="K39" s="30"/>
@@ -2068,12 +2053,12 @@
         <v>1</v>
       </c>
       <c r="H40" s="49">
-        <f t="shared" si="0"/>
-        <v>45184</v>
+        <f t="shared" si="3"/>
+        <v>45157</v>
       </c>
       <c r="I40" s="49">
-        <f t="shared" si="4"/>
-        <v>45185</v>
+        <f t="shared" si="5"/>
+        <v>45158</v>
       </c>
       <c r="J40" s="30"/>
       <c r="K40" s="30"/>
@@ -2094,12 +2079,12 @@
         <v>1</v>
       </c>
       <c r="H41" s="49">
-        <f t="shared" si="0"/>
-        <v>45186</v>
+        <f t="shared" si="3"/>
+        <v>45159</v>
       </c>
       <c r="I41" s="49">
-        <f t="shared" si="4"/>
-        <v>45187</v>
+        <f t="shared" si="5"/>
+        <v>45160</v>
       </c>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
@@ -2122,12 +2107,12 @@
         <v>3</v>
       </c>
       <c r="H42" s="49">
-        <f t="shared" si="0"/>
-        <v>45188</v>
+        <f t="shared" si="3"/>
+        <v>45161</v>
       </c>
       <c r="I42" s="49">
-        <f t="shared" si="4"/>
-        <v>45191</v>
+        <f t="shared" si="5"/>
+        <v>45164</v>
       </c>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
@@ -2150,12 +2135,12 @@
         <v>5</v>
       </c>
       <c r="H43" s="49">
-        <f t="shared" si="0"/>
-        <v>45192</v>
+        <f t="shared" si="3"/>
+        <v>45165</v>
       </c>
       <c r="I43" s="49">
-        <f t="shared" si="4"/>
-        <v>45197</v>
+        <f t="shared" si="5"/>
+        <v>45170</v>
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="35"/>

</xml_diff>

<commit_message>
Added network hyper params table
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED1DB0F-90B0-4053-B1BC-12A26CC945D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB93CE81-D8BB-4E4A-A578-6FFF25AC280B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -257,6 +268,9 @@
   </si>
   <si>
     <t>RL note</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -266,7 +280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +372,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,7 +427,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,10 +509,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -646,16 +682,26 @@
     <xf numFmtId="16" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -989,9 +1035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B960D0FC-F9A3-469E-ABD5-093C4BA06CC0}">
   <dimension ref="B1:M43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1045,7 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="1.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="41.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" style="48" customWidth="1"/>
@@ -1031,9 +1077,9 @@
       </c>
       <c r="L1" s="50">
         <f ca="1">TODAY()</f>
-        <v>45123</v>
-      </c>
-      <c r="M1" s="55"/>
+        <v>45125</v>
+      </c>
+      <c r="M1" s="68"/>
     </row>
     <row r="2" spans="2:13" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C2" s="15"/>
@@ -1044,17 +1090,22 @@
       </c>
       <c r="H2" s="54">
         <f>SUM($G$4:$G$43)</f>
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>70</v>
       </c>
       <c r="J2" s="67">
         <f ca="1">L1+H2+5</f>
-        <v>45168</v>
-      </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="50"/>
+        <v>45159</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="69">
+        <f>(H1-H2)/H1</f>
+        <v>0.47272727272727272</v>
+      </c>
       <c r="M2" s="55"/>
     </row>
     <row r="3" spans="2:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -1334,23 +1385,23 @@
       <c r="D13" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="66">
         <v>0</v>
       </c>
-      <c r="H13" s="69">
+      <c r="H13" s="49">
         <f>I12+1</f>
         <v>45122</v>
       </c>
-      <c r="I13" s="69">
+      <c r="I13" s="49">
         <f t="shared" si="0"/>
         <v>45122</v>
       </c>
-      <c r="J13" s="69">
+      <c r="J13" s="49">
         <v>45120</v>
       </c>
-      <c r="K13" s="69">
+      <c r="K13" s="49">
         <v>45121</v>
       </c>
       <c r="L13" s="31"/>
@@ -1396,15 +1447,15 @@
       </c>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
-      <c r="G15" s="41">
-        <v>2</v>
+      <c r="G15" s="66">
+        <v>0</v>
       </c>
       <c r="H15" s="49">
         <v>45118</v>
       </c>
       <c r="I15" s="49">
         <f t="shared" si="0"/>
-        <v>45120</v>
+        <v>45118</v>
       </c>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
@@ -1460,8 +1511,12 @@
         <f t="shared" si="1"/>
         <v>45120</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="49">
+        <v>45121</v>
+      </c>
+      <c r="K17" s="49">
+        <v>45123</v>
+      </c>
       <c r="L17" s="31"/>
       <c r="M17" s="58">
         <v>1</v>
@@ -1485,8 +1540,12 @@
         <f t="shared" si="1"/>
         <v>45121</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
+      <c r="J18" s="49">
+        <v>45121</v>
+      </c>
+      <c r="K18" s="49">
+        <v>45123</v>
+      </c>
       <c r="L18" s="31"/>
       <c r="M18" s="58">
         <v>1</v>
@@ -1495,20 +1554,20 @@
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="31" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="31"/>
-      <c r="G19" s="41">
-        <v>1</v>
+      <c r="G19" s="66">
+        <v>0</v>
       </c>
       <c r="H19" s="49">
         <v>45122</v>
       </c>
       <c r="I19" s="49">
         <f t="shared" si="1"/>
-        <v>45123</v>
+        <v>45122</v>
       </c>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
@@ -1521,22 +1580,26 @@
       <c r="B20" s="34"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="70" t="s">
+      <c r="E20" s="53" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="53"/>
-      <c r="G20" s="41">
-        <v>1</v>
+      <c r="G20" s="66">
+        <v>0</v>
       </c>
       <c r="H20" s="49">
         <v>45123</v>
       </c>
       <c r="I20" s="49">
         <f t="shared" si="1"/>
+        <v>45123</v>
+      </c>
+      <c r="J20" s="49">
         <v>45124</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
+      <c r="K20" s="49">
+        <v>45124</v>
+      </c>
       <c r="L20" s="31"/>
       <c r="M20" s="58">
         <v>1</v>
@@ -1550,18 +1613,22 @@
         <v>7</v>
       </c>
       <c r="F21" s="53"/>
-      <c r="G21" s="41">
-        <v>1</v>
+      <c r="G21" s="66">
+        <v>0</v>
       </c>
       <c r="H21" s="49">
         <v>45124</v>
       </c>
       <c r="I21" s="49">
         <f t="shared" si="1"/>
-        <v>45125</v>
-      </c>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+        <v>45124</v>
+      </c>
+      <c r="J21" s="49">
+        <v>45124</v>
+      </c>
+      <c r="K21" s="49">
+        <v>45124</v>
+      </c>
       <c r="L21" s="31"/>
       <c r="M21" s="58">
         <v>1</v>
@@ -1575,18 +1642,22 @@
         <v>71</v>
       </c>
       <c r="F22" s="53"/>
-      <c r="G22" s="41">
-        <v>1</v>
+      <c r="G22" s="66">
+        <v>0</v>
       </c>
       <c r="H22" s="49">
         <v>45125</v>
       </c>
       <c r="I22" s="49">
         <f t="shared" si="1"/>
-        <v>45126</v>
-      </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
+        <v>45125</v>
+      </c>
+      <c r="J22" s="49">
+        <v>45124</v>
+      </c>
+      <c r="K22" s="49">
+        <v>45124</v>
+      </c>
       <c r="L22" s="31"/>
       <c r="M22" s="58">
         <v>1</v>
@@ -1600,18 +1671,22 @@
         <v>73</v>
       </c>
       <c r="F23" s="53"/>
-      <c r="G23" s="41">
-        <v>1</v>
+      <c r="G23" s="66">
+        <v>0</v>
       </c>
       <c r="H23" s="49">
         <v>45126</v>
       </c>
       <c r="I23" s="49">
         <f t="shared" si="1"/>
-        <v>45127</v>
-      </c>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
+        <v>45126</v>
+      </c>
+      <c r="J23" s="49">
+        <v>45124</v>
+      </c>
+      <c r="K23" s="49">
+        <v>45124</v>
+      </c>
       <c r="L23" s="31"/>
       <c r="M23" s="58">
         <v>1</v>
@@ -1625,18 +1700,22 @@
         <v>74</v>
       </c>
       <c r="F24" s="53"/>
-      <c r="G24" s="41">
-        <v>1</v>
+      <c r="G24" s="66">
+        <v>0</v>
       </c>
       <c r="H24" s="49">
         <v>45127</v>
       </c>
       <c r="I24" s="49">
         <f t="shared" si="1"/>
-        <v>45128</v>
-      </c>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
+        <v>45127</v>
+      </c>
+      <c r="J24" s="49">
+        <v>45124</v>
+      </c>
+      <c r="K24" s="49">
+        <v>45124</v>
+      </c>
       <c r="L24" s="31"/>
       <c r="M24" s="58">
         <v>1</v>
@@ -1646,22 +1725,26 @@
       <c r="B25" s="34"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="53" t="s">
         <v>72</v>
       </c>
       <c r="F25" s="53"/>
-      <c r="G25" s="41">
-        <v>1</v>
+      <c r="G25" s="66">
+        <v>0</v>
       </c>
       <c r="H25" s="49">
         <v>45128</v>
       </c>
       <c r="I25" s="49">
         <f t="shared" si="1"/>
-        <v>45129</v>
-      </c>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
+        <v>45128</v>
+      </c>
+      <c r="J25" s="49">
+        <v>45123</v>
+      </c>
+      <c r="K25" s="49">
+        <v>45123</v>
+      </c>
       <c r="L25" s="31"/>
       <c r="M25" s="58">
         <v>1</v>
@@ -1670,23 +1753,25 @@
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="34"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="53" t="s">
+      <c r="D26" s="70"/>
+      <c r="E26" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="53"/>
-      <c r="G26" s="41">
-        <v>1</v>
-      </c>
+      <c r="F26" s="72"/>
+      <c r="G26" s="73"/>
       <c r="H26" s="49">
         <v>45129</v>
       </c>
       <c r="I26" s="49">
         <f t="shared" si="1"/>
-        <v>45130</v>
-      </c>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
+        <v>45129</v>
+      </c>
+      <c r="J26" s="49">
+        <v>45125</v>
+      </c>
+      <c r="K26" s="49">
+        <v>45125</v>
+      </c>
       <c r="L26" s="31"/>
       <c r="M26" s="58">
         <v>1</v>
@@ -1696,19 +1781,19 @@
       <c r="B27" s="34"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="53" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="53"/>
-      <c r="G27" s="41">
-        <v>1</v>
+      <c r="G27" s="66">
+        <v>0</v>
       </c>
       <c r="H27" s="49">
         <v>45130</v>
       </c>
       <c r="I27" s="49">
         <f t="shared" si="1"/>
-        <v>45131</v>
+        <v>45130</v>
       </c>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
@@ -1720,7 +1805,7 @@
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="34"/>
       <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="18" t="s">
         <v>15</v>
       </c>
@@ -2216,7 +2301,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">TODAY()+D37</f>
-        <v>45154.5</v>
+        <v>45156.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Results section - Started
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB93CE81-D8BB-4E4A-A578-6FFF25AC280B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F6BC22-45C8-4BF2-B1A3-0050E14B5819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>Look ahead parameter + env_test with WT_ORG</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -280,7 +286,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,8 +393,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,12 +447,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -508,12 +528,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -691,13 +720,43 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,11 +1092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B960D0FC-F9A3-469E-ABD5-093C4BA06CC0}">
-  <dimension ref="B1:M43"/>
+  <dimension ref="B1:M44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,8 +1122,8 @@
         <v>67</v>
       </c>
       <c r="H1" s="54">
-        <f>SUM(M4:M43)</f>
-        <v>55</v>
+        <f>SUM(M4:M44)</f>
+        <v>56</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>51</v>
@@ -1077,7 +1136,7 @@
       </c>
       <c r="L1" s="50">
         <f ca="1">TODAY()</f>
-        <v>45125</v>
+        <v>45127</v>
       </c>
       <c r="M1" s="68"/>
     </row>
@@ -1089,22 +1148,22 @@
         <v>68</v>
       </c>
       <c r="H2" s="54">
-        <f>SUM($G$4:$G$43)</f>
-        <v>29</v>
+        <f>SUM($G$4:$G$44)</f>
+        <v>14</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>70</v>
       </c>
       <c r="J2" s="67">
-        <f ca="1">L1+H2+5</f>
-        <v>45159</v>
+        <f ca="1">L1+H2+20%*(H2)</f>
+        <v>45143.8</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>77</v>
       </c>
       <c r="L2" s="69">
         <f>(H1-H2)/H1</f>
-        <v>0.47272727272727272</v>
+        <v>0.75</v>
       </c>
       <c r="M2" s="55"/>
     </row>
@@ -1419,8 +1478,8 @@
       <c r="D14" s="36"/>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
-      <c r="G14" s="41">
-        <v>2</v>
+      <c r="G14" s="66">
+        <v>0</v>
       </c>
       <c r="H14" s="49">
         <f>I13+1</f>
@@ -1428,7 +1487,7 @@
       </c>
       <c r="I14" s="49">
         <f t="shared" si="0"/>
-        <v>45125</v>
+        <v>45123</v>
       </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
@@ -1554,7 +1613,7 @@
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="71"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="31" t="s">
         <v>1</v>
       </c>
@@ -1754,11 +1813,11 @@
       <c r="B26" s="34"/>
       <c r="C26" s="18"/>
       <c r="D26" s="70"/>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="72"/>
-      <c r="G26" s="73"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="72"/>
       <c r="H26" s="49">
         <v>45129</v>
       </c>
@@ -1837,18 +1896,22 @@
       </c>
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
-      <c r="G29" s="41">
-        <v>2</v>
+      <c r="G29" s="66">
+        <v>0</v>
       </c>
       <c r="H29" s="49">
         <v>45130</v>
       </c>
       <c r="I29" s="49">
         <f t="shared" ref="I29" si="2">H29+G29</f>
-        <v>45132</v>
-      </c>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
+        <v>45130</v>
+      </c>
+      <c r="J29" s="49">
+        <v>45125</v>
+      </c>
+      <c r="K29" s="49">
+        <v>45126</v>
+      </c>
       <c r="L29" s="31"/>
       <c r="M29" s="58">
         <v>2</v>
@@ -1864,16 +1927,16 @@
       </c>
       <c r="E30" s="44"/>
       <c r="F30" s="44"/>
-      <c r="G30" s="41">
-        <v>2</v>
+      <c r="G30" s="66">
+        <v>0</v>
       </c>
       <c r="H30" s="49">
-        <f t="shared" ref="H30:H43" si="3">I29+1</f>
-        <v>45133</v>
+        <f t="shared" ref="H30:H42" si="3">I29+1</f>
+        <v>45131</v>
       </c>
       <c r="I30" s="49">
         <f t="shared" ref="I30" si="4">H30+G30</f>
-        <v>45135</v>
+        <v>45131</v>
       </c>
       <c r="J30" s="30"/>
       <c r="K30" s="30"/>
@@ -1890,19 +1953,23 @@
         <v>65</v>
       </c>
       <c r="F31" s="44"/>
-      <c r="G31" s="41">
-        <v>1</v>
+      <c r="G31" s="66">
+        <v>0</v>
       </c>
       <c r="H31" s="49">
         <f t="shared" si="3"/>
-        <v>45136</v>
+        <v>45132</v>
       </c>
       <c r="I31" s="49">
-        <f t="shared" ref="I31:I43" si="5">H31+G31</f>
-        <v>45137</v>
-      </c>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
+        <f t="shared" ref="I31:I44" si="5">H31+G31</f>
+        <v>45132</v>
+      </c>
+      <c r="J31" s="49">
+        <v>45126</v>
+      </c>
+      <c r="K31" s="49">
+        <v>45126</v>
+      </c>
       <c r="L31" s="31"/>
       <c r="M31" s="58">
         <v>1</v>
@@ -1916,19 +1983,23 @@
         <v>66</v>
       </c>
       <c r="F32" s="44"/>
-      <c r="G32" s="41">
-        <v>1</v>
+      <c r="G32" s="66">
+        <v>0</v>
       </c>
       <c r="H32" s="49">
         <f t="shared" si="3"/>
-        <v>45138</v>
+        <v>45133</v>
       </c>
       <c r="I32" s="49">
         <f t="shared" si="5"/>
-        <v>45139</v>
-      </c>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
+        <v>45133</v>
+      </c>
+      <c r="J32" s="49">
+        <v>45126</v>
+      </c>
+      <c r="K32" s="49">
+        <v>45126</v>
+      </c>
       <c r="L32" s="31"/>
       <c r="M32" s="58">
         <v>1</v>
@@ -1944,19 +2015,23 @@
       </c>
       <c r="E33" s="44"/>
       <c r="F33" s="44"/>
-      <c r="G33" s="41">
-        <v>1</v>
+      <c r="G33" s="66">
+        <v>0</v>
       </c>
       <c r="H33" s="49">
         <f t="shared" si="3"/>
-        <v>45140</v>
+        <v>45134</v>
       </c>
       <c r="I33" s="49">
         <f t="shared" si="5"/>
-        <v>45141</v>
-      </c>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
+        <v>45134</v>
+      </c>
+      <c r="J33" s="49">
+        <v>45126</v>
+      </c>
+      <c r="K33" s="49">
+        <v>45127</v>
+      </c>
       <c r="L33" s="31"/>
       <c r="M33" s="58">
         <v>1</v>
@@ -1970,19 +2045,23 @@
         <v>11</v>
       </c>
       <c r="F34" s="44"/>
-      <c r="G34" s="41">
-        <v>1</v>
+      <c r="G34" s="66">
+        <v>0</v>
       </c>
       <c r="H34" s="49">
         <f t="shared" si="3"/>
-        <v>45142</v>
+        <v>45135</v>
       </c>
       <c r="I34" s="49">
         <f t="shared" si="5"/>
-        <v>45143</v>
-      </c>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+        <v>45135</v>
+      </c>
+      <c r="J34" s="49">
+        <v>45127</v>
+      </c>
+      <c r="K34" s="49">
+        <v>45127</v>
+      </c>
       <c r="L34" s="31"/>
       <c r="M34" s="58">
         <v>1</v>
@@ -1996,19 +2075,23 @@
         <v>12</v>
       </c>
       <c r="F35" s="44"/>
-      <c r="G35" s="41">
-        <v>0.5</v>
+      <c r="G35" s="66">
+        <v>0</v>
       </c>
       <c r="H35" s="49">
         <f t="shared" si="3"/>
-        <v>45144</v>
+        <v>45136</v>
       </c>
       <c r="I35" s="49">
         <f t="shared" si="5"/>
-        <v>45144.5</v>
-      </c>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
+        <v>45136</v>
+      </c>
+      <c r="J35" s="49">
+        <v>45127</v>
+      </c>
+      <c r="K35" s="49">
+        <v>45127</v>
+      </c>
       <c r="L35" s="31"/>
       <c r="M35" s="58">
         <v>0.5</v>
@@ -2022,19 +2105,23 @@
         <v>13</v>
       </c>
       <c r="F36" s="44"/>
-      <c r="G36" s="41">
-        <v>0.5</v>
+      <c r="G36" s="66">
+        <v>0</v>
       </c>
       <c r="H36" s="49">
         <f t="shared" si="3"/>
-        <v>45145.5</v>
+        <v>45137</v>
       </c>
       <c r="I36" s="49">
         <f t="shared" si="5"/>
-        <v>45146</v>
-      </c>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
+        <v>45137</v>
+      </c>
+      <c r="J36" s="49">
+        <v>45127</v>
+      </c>
+      <c r="K36" s="49">
+        <v>45127</v>
+      </c>
       <c r="L36" s="31"/>
       <c r="M36" s="58">
         <v>0.5</v>
@@ -2050,16 +2137,16 @@
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
       <c r="F37" s="44"/>
-      <c r="G37" s="41">
-        <v>4</v>
+      <c r="G37" s="66">
+        <v>0</v>
       </c>
       <c r="H37" s="49">
         <f t="shared" si="3"/>
-        <v>45147</v>
+        <v>45138</v>
       </c>
       <c r="I37" s="49">
         <f t="shared" si="5"/>
-        <v>45151</v>
+        <v>45138</v>
       </c>
       <c r="J37" s="30"/>
       <c r="K37" s="30"/>
@@ -2079,15 +2166,15 @@
       <c r="E38" s="18"/>
       <c r="F38" s="44"/>
       <c r="G38" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38" s="49">
         <f t="shared" si="3"/>
-        <v>45152</v>
+        <v>45139</v>
       </c>
       <c r="I38" s="49">
         <f t="shared" si="5"/>
-        <v>45154</v>
+        <v>45140</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
@@ -2109,11 +2196,11 @@
       </c>
       <c r="H39" s="49">
         <f t="shared" si="3"/>
-        <v>45155</v>
+        <v>45141</v>
       </c>
       <c r="I39" s="49">
         <f t="shared" si="5"/>
-        <v>45156</v>
+        <v>45142</v>
       </c>
       <c r="J39" s="30"/>
       <c r="K39" s="30"/>
@@ -2124,26 +2211,30 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="34"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="18" t="s">
+      <c r="C40" s="81"/>
+      <c r="D40" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="41">
-        <v>1</v>
-      </c>
-      <c r="H40" s="49">
+      <c r="E40" s="82"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="84">
+        <v>1</v>
+      </c>
+      <c r="H40" s="85">
         <f t="shared" si="3"/>
-        <v>45157</v>
-      </c>
-      <c r="I40" s="49">
+        <v>45143</v>
+      </c>
+      <c r="I40" s="85">
         <f t="shared" si="5"/>
+        <v>45144</v>
+      </c>
+      <c r="J40" s="85">
         <v>45158</v>
       </c>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="31"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="87" t="s">
+        <v>79</v>
+      </c>
       <c r="M40" s="58">
         <v>1</v>
       </c>
@@ -2161,11 +2252,11 @@
       </c>
       <c r="H41" s="49">
         <f t="shared" si="3"/>
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="I41" s="49">
         <f t="shared" si="5"/>
-        <v>45160</v>
+        <v>45146</v>
       </c>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
@@ -2189,11 +2280,11 @@
       </c>
       <c r="H42" s="49">
         <f t="shared" si="3"/>
-        <v>45161</v>
+        <v>45147</v>
       </c>
       <c r="I42" s="49">
         <f t="shared" si="5"/>
-        <v>45164</v>
+        <v>45150</v>
       </c>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
@@ -2203,30 +2294,52 @@
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="38">
+      <c r="B43" s="80">
         <v>8</v>
       </c>
-      <c r="C43" s="51" t="s">
+      <c r="C43" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="79">
+        <v>1</v>
+      </c>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="74"/>
+      <c r="M43" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="38">
+        <v>9</v>
+      </c>
+      <c r="C44" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="42">
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="42">
         <v>5</v>
       </c>
-      <c r="H43" s="49">
-        <f t="shared" si="3"/>
-        <v>45165</v>
-      </c>
-      <c r="I43" s="49">
+      <c r="H44" s="49">
+        <f>I42+1</f>
+        <v>45151</v>
+      </c>
+      <c r="I44" s="49">
         <f t="shared" si="5"/>
-        <v>45170</v>
-      </c>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="59">
+        <v>45156</v>
+      </c>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="59">
         <v>5</v>
       </c>
     </row>
@@ -2301,7 +2414,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">TODAY()+D37</f>
-        <v>45156.5</v>
+        <v>45158.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Artcile added results. Only discussion and conculsion remain
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F6BC22-45C8-4BF2-B1A3-0050E14B5819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80DB72E-17FD-46EB-855B-C94177BE044E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -201,9 +190,6 @@
     <t>A. end</t>
   </si>
   <si>
-    <t>Experiments</t>
-  </si>
-  <si>
     <t>Plots</t>
   </si>
   <si>
@@ -276,7 +262,10 @@
     <t>Look ahead parameter + env_test with WT_ORG</t>
   </si>
   <si>
-    <t>WIP</t>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Discussion</t>
   </si>
 </sst>
 </file>
@@ -402,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,12 +437,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -742,19 +725,18 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -1096,7 +1078,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1101,7 @@
       <c r="D1" s="15"/>
       <c r="F1" s="62"/>
       <c r="G1" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H1" s="54">
         <f>SUM(M4:M44)</f>
@@ -1132,11 +1114,11 @@
         <v>45184</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L1" s="50">
         <f ca="1">TODAY()</f>
-        <v>45127</v>
+        <v>45129</v>
       </c>
       <c r="M1" s="68"/>
     </row>
@@ -1145,25 +1127,25 @@
       <c r="D2" s="15"/>
       <c r="F2" s="62"/>
       <c r="G2" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="54">
         <f>SUM($G$4:$G$44)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I2" s="61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="67">
         <f ca="1">L1+H2+20%*(H2)</f>
-        <v>45143.8</v>
+        <v>45142.2</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L2" s="69">
         <f>(H1-H2)/H1</f>
-        <v>0.75</v>
+        <v>0.8035714285714286</v>
       </c>
       <c r="M2" s="55"/>
     </row>
@@ -1196,7 +1178,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -1279,7 +1261,7 @@
       <c r="B7" s="34"/>
       <c r="C7" s="36"/>
       <c r="D7" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
@@ -1307,7 +1289,7 @@
       <c r="B8" s="34"/>
       <c r="C8" s="36"/>
       <c r="D8" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
@@ -1337,7 +1319,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="31"/>
@@ -1356,7 +1338,7 @@
         <v>3.1</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
@@ -1386,7 +1368,7 @@
       <c r="B11" s="34"/>
       <c r="C11" s="18"/>
       <c r="D11" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
@@ -1416,7 +1398,7 @@
       <c r="B12" s="34"/>
       <c r="C12" s="18"/>
       <c r="D12" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
@@ -1502,7 +1484,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
@@ -1698,7 +1680,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="66">
@@ -1727,7 +1709,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="66">
@@ -1756,7 +1738,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="66">
@@ -1785,7 +1767,7 @@
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25" s="53"/>
       <c r="G25" s="66">
@@ -1814,7 +1796,7 @@
       <c r="C26" s="18"/>
       <c r="D26" s="70"/>
       <c r="E26" s="71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26" s="71"/>
       <c r="G26" s="72"/>
@@ -1950,7 +1932,7 @@
       <c r="C31" s="31"/>
       <c r="D31" s="36"/>
       <c r="E31" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="44"/>
       <c r="G31" s="66">
@@ -1980,7 +1962,7 @@
       <c r="C32" s="31"/>
       <c r="D32" s="36"/>
       <c r="E32" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F32" s="44"/>
       <c r="G32" s="66">
@@ -2132,7 +2114,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
@@ -2148,8 +2130,12 @@
         <f t="shared" si="5"/>
         <v>45138</v>
       </c>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
+      <c r="J37" s="84">
+        <v>45158</v>
+      </c>
+      <c r="K37" s="84">
+        <v>45129</v>
+      </c>
       <c r="L37" s="31"/>
       <c r="M37" s="58">
         <v>4</v>
@@ -2160,13 +2146,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="44"/>
       <c r="G38" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38" s="49">
         <f t="shared" si="3"/>
@@ -2174,7 +2160,7 @@
       </c>
       <c r="I38" s="49">
         <f t="shared" si="5"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
@@ -2185,26 +2171,26 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="34"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="41">
-        <v>1</v>
-      </c>
-      <c r="H39" s="49">
+      <c r="C39" s="81"/>
+      <c r="D39" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="82"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="66">
+        <v>0</v>
+      </c>
+      <c r="H39" s="84">
         <f t="shared" si="3"/>
-        <v>45141</v>
-      </c>
-      <c r="I39" s="49">
+        <v>45142</v>
+      </c>
+      <c r="I39" s="84">
         <f t="shared" si="5"/>
         <v>45142</v>
       </c>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="31"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="86"/>
       <c r="M39" s="58">
         <v>1</v>
       </c>
@@ -2213,54 +2199,50 @@
       <c r="B40" s="34"/>
       <c r="C40" s="81"/>
       <c r="D40" s="82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" s="82"/>
       <c r="F40" s="83"/>
-      <c r="G40" s="84">
-        <v>1</v>
-      </c>
-      <c r="H40" s="85">
+      <c r="G40" s="66">
+        <v>0</v>
+      </c>
+      <c r="H40" s="84">
         <f t="shared" si="3"/>
         <v>45143</v>
       </c>
-      <c r="I40" s="85">
+      <c r="I40" s="84">
+        <f t="shared" si="5"/>
+        <v>45143</v>
+      </c>
+      <c r="J40" s="84"/>
+      <c r="K40" s="84"/>
+      <c r="L40" s="86"/>
+      <c r="M40" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="34"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="82" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="82"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="66">
+        <v>0</v>
+      </c>
+      <c r="H41" s="84">
+        <f t="shared" si="3"/>
+        <v>45144</v>
+      </c>
+      <c r="I41" s="84">
         <f t="shared" si="5"/>
         <v>45144</v>
       </c>
-      <c r="J40" s="85">
-        <v>45158</v>
-      </c>
-      <c r="K40" s="86"/>
-      <c r="L40" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="M40" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="34"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="41">
-        <v>1</v>
-      </c>
-      <c r="H41" s="49">
-        <f t="shared" si="3"/>
-        <v>45145</v>
-      </c>
-      <c r="I41" s="49">
-        <f t="shared" si="5"/>
-        <v>45146</v>
-      </c>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="31"/>
+      <c r="J41" s="85"/>
+      <c r="K41" s="85"/>
+      <c r="L41" s="86"/>
       <c r="M41" s="58">
         <v>1</v>
       </c>
@@ -2276,15 +2258,15 @@
       <c r="E42" s="18"/>
       <c r="F42" s="44"/>
       <c r="G42" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H42" s="49">
         <f t="shared" si="3"/>
-        <v>45147</v>
+        <v>45145</v>
       </c>
       <c r="I42" s="49">
         <f t="shared" si="5"/>
-        <v>45150</v>
+        <v>45147</v>
       </c>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
@@ -2298,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D43" s="77"/>
       <c r="E43" s="77"/>
@@ -2320,7 +2302,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" s="37"/>
       <c r="E44" s="37"/>
@@ -2330,11 +2312,11 @@
       </c>
       <c r="H44" s="49">
         <f>I42+1</f>
-        <v>45151</v>
+        <v>45148</v>
       </c>
       <c r="I44" s="49">
         <f t="shared" si="5"/>
-        <v>45156</v>
+        <v>45153</v>
       </c>
       <c r="J44" s="35"/>
       <c r="K44" s="35"/>
@@ -2414,7 +2396,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">TODAY()+D37</f>
-        <v>45158.5</v>
+        <v>45160.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Article -- Added discussion section elements
</commit_message>
<xml_diff>
--- a/article_plan.xlsx
+++ b/article_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80DB72E-17FD-46EB-855B-C94177BE044E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A1A030-12D2-4420-8832-C872351B1DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>Update performance tables</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>Discussion</t>
+  </si>
+  <si>
+    <t>General discussions</t>
+  </si>
+  <si>
+    <t>Summary - results and plots and t-tests</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -725,19 +731,14 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1078,7 +1079,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1119,7 @@
       </c>
       <c r="L1" s="50">
         <f ca="1">TODAY()</f>
-        <v>45129</v>
+        <v>45130</v>
       </c>
       <c r="M1" s="68"/>
     </row>
@@ -1131,21 +1132,21 @@
       </c>
       <c r="H2" s="54">
         <f>SUM($G$4:$G$44)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>69</v>
       </c>
       <c r="J2" s="67">
         <f ca="1">L1+H2+20%*(H2)</f>
-        <v>45142.2</v>
+        <v>45140.800000000003</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>76</v>
       </c>
       <c r="L2" s="69">
         <f>(H1-H2)/H1</f>
-        <v>0.8035714285714286</v>
+        <v>0.8392857142857143</v>
       </c>
       <c r="M2" s="55"/>
     </row>
@@ -1844,25 +1845,29 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
-      <c r="C28" s="18"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="82"/>
       <c r="D28" s="70"/>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="53"/>
-      <c r="G28" s="41">
-        <v>1</v>
+      <c r="F28" s="83"/>
+      <c r="G28" s="66">
+        <v>0</v>
       </c>
       <c r="H28" s="49">
         <v>45131</v>
       </c>
       <c r="I28" s="49">
         <f t="shared" si="1"/>
-        <v>45132</v>
-      </c>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
+        <v>45131</v>
+      </c>
+      <c r="J28" s="49">
+        <v>45130</v>
+      </c>
+      <c r="K28" s="49">
+        <v>45130</v>
+      </c>
       <c r="L28" s="31"/>
       <c r="M28" s="58">
         <v>1</v>
@@ -2130,10 +2135,10 @@
         <f t="shared" si="5"/>
         <v>45138</v>
       </c>
-      <c r="J37" s="84">
+      <c r="J37" s="49">
         <v>45158</v>
       </c>
-      <c r="K37" s="84">
+      <c r="K37" s="49">
         <v>45129</v>
       </c>
       <c r="L37" s="31"/>
@@ -2151,16 +2156,14 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="44"/>
-      <c r="G38" s="41">
-        <v>2</v>
-      </c>
+      <c r="G38" s="41"/>
       <c r="H38" s="49">
         <f t="shared" si="3"/>
         <v>45139</v>
       </c>
       <c r="I38" s="49">
         <f t="shared" si="5"/>
-        <v>45141</v>
+        <v>45139</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
@@ -2171,78 +2174,72 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="34"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="82" t="s">
+      <c r="C39" s="46"/>
+      <c r="D39" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="82"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="66">
-        <v>0</v>
-      </c>
-      <c r="H39" s="84">
+      <c r="E39" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="44"/>
+      <c r="G39" s="79">
+        <v>2</v>
+      </c>
+      <c r="H39" s="49">
         <f t="shared" si="3"/>
-        <v>45142</v>
-      </c>
-      <c r="I39" s="84">
+        <v>45140</v>
+      </c>
+      <c r="I39" s="49">
         <f t="shared" si="5"/>
         <v>45142</v>
       </c>
-      <c r="J39" s="85"/>
-      <c r="K39" s="85"/>
-      <c r="L39" s="86"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="31"/>
       <c r="M39" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="34"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="82" t="s">
+      <c r="C40" s="46"/>
+      <c r="D40" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="82"/>
-      <c r="F40" s="83"/>
+      <c r="E40" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="44"/>
       <c r="G40" s="66">
         <v>0</v>
       </c>
-      <c r="H40" s="84">
+      <c r="H40" s="49">
         <f t="shared" si="3"/>
         <v>45143</v>
       </c>
-      <c r="I40" s="84">
+      <c r="I40" s="49">
         <f t="shared" si="5"/>
         <v>45143</v>
       </c>
-      <c r="J40" s="84"/>
-      <c r="K40" s="84"/>
-      <c r="L40" s="86"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="31"/>
       <c r="M40" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="34"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="82"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="66">
-        <v>0</v>
-      </c>
-      <c r="H41" s="84">
-        <f t="shared" si="3"/>
-        <v>45144</v>
-      </c>
-      <c r="I41" s="84">
-        <f t="shared" si="5"/>
-        <v>45144</v>
-      </c>
-      <c r="J41" s="85"/>
-      <c r="K41" s="85"/>
-      <c r="L41" s="86"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="31"/>
       <c r="M41" s="58">
         <v>1</v>
       </c>
@@ -2261,12 +2258,12 @@
         <v>2</v>
       </c>
       <c r="H42" s="49">
-        <f t="shared" si="3"/>
-        <v>45145</v>
+        <f>I40+1</f>
+        <v>45144</v>
       </c>
       <c r="I42" s="49">
         <f t="shared" si="5"/>
-        <v>45147</v>
+        <v>45146</v>
       </c>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
@@ -2308,15 +2305,15 @@
       <c r="E44" s="37"/>
       <c r="F44" s="37"/>
       <c r="G44" s="42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H44" s="49">
         <f>I42+1</f>
-        <v>45148</v>
+        <v>45147</v>
       </c>
       <c r="I44" s="49">
         <f t="shared" si="5"/>
-        <v>45153</v>
+        <v>45151</v>
       </c>
       <c r="J44" s="35"/>
       <c r="K44" s="35"/>
@@ -2396,7 +2393,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">TODAY()+D37</f>
-        <v>45160.5</v>
+        <v>45161.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>